<commit_message>
Products page tests have been added
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zaliczenie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shopTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320DC9F2-7B31-4A21-A6E5-9F821B469E53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FDB16B-997D-4535-A0E7-15FDFA5A8294}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Użytkownik widzi napis z nazwą wcześniej dodanego do koszyka produktu</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -217,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -281,11 +284,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -325,6 +339,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,7 +678,7 @@
     <col min="8" max="8" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -674,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -682,7 +702,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -690,13 +710,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -704,8 +724,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -731,7 +751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>1</v>
       </c>
@@ -756,8 +776,11 @@
       <c r="H10" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="I10" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>2</v>
       </c>
@@ -782,8 +805,11 @@
       <c r="H11" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I11" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>3</v>
       </c>
@@ -808,8 +834,11 @@
       <c r="H12" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I12" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>4</v>
       </c>
@@ -834,8 +863,11 @@
       <c r="H13" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="I13" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>5</v>
       </c>
@@ -859,6 +891,9 @@
       </c>
       <c r="H14" s="11" t="s">
         <v>46</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.3">

</xml_diff>